<commit_message>
updated info about Rayyan
</commit_message>
<xml_diff>
--- a/files/SLR Tools Analysis.xlsx
+++ b/files/SLR Tools Analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aas358/Development/ai-slr/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE398F1-3AC2-BE4E-AC7D-18CC882E1005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B9384A-060E-C64C-8B89-C6226593F9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SLR AI Features for Screening" sheetId="1" r:id="rId1"/>
@@ -361,11 +361,6 @@
   <si>
     <t>Relevant papers: 5.
 Irrelevant papers: 5.</t>
-  </si>
-  <si>
-    <t>Keywords search: It searches by keywords that could be highlighted;
- Other searches: It searches by author or publication year;
- Boolean Operator: It searches by the combination of boolean operators(AND, OR, NOT) with keywords.</t>
   </si>
   <si>
     <t>Research Screener</t>
@@ -758,6 +753,15 @@
   <si>
     <t>NA: Not applicable because the tools are specifically for extraction</t>
   </si>
+  <si>
+    <t>Keywords search: It searches by keywords that could be highlighted;
+ Other searches: It searches by author or publication year;
+ Boolean Operator: It searches by the combination of boolean operators(AND, OR, NOT) with keywords.
+PICO identification: Highlights the parts of a PICO question in the abstract.
+Location facet: Extracts the study locations (highly applicable in  biomedical studies).
+Tpoics: Extracts topics enriching them with MeSH terms.
+Biomedical keywords: Prepopulates a set of  keywords and phrases (highly applicable in RCT).</t>
+  </si>
 </sst>
 </file>
 
@@ -820,7 +824,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -829,7 +833,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1060,9 +1063,9 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:L20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1077,40 +1080,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="42" x14ac:dyDescent="0.15">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="1"/>
@@ -1493,7 +1496,7 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="319" x14ac:dyDescent="0.15">
-      <c r="A9" s="4" t="s">
+      <c r="A9" t="s">
         <v>63</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1752,7 +1755,7 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="1:26" ht="112" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:26" ht="266" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>92</v>
       </c>
@@ -1784,7 +1787,7 @@
         <v>29</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>96</v>
+        <v>220</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>23</v>
@@ -1806,7 +1809,7 @@
     </row>
     <row r="15" spans="1:26" ht="84" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>13</v>
@@ -1818,19 +1821,19 @@
         <v>15</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>18</v>
       </c>
       <c r="H15" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>29</v>
@@ -1858,7 +1861,7 @@
     </row>
     <row r="16" spans="1:26" ht="168" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>13</v>
@@ -1879,7 +1882,7 @@
         <v>18</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>20</v>
@@ -1888,7 +1891,7 @@
         <v>29</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>23</v>
@@ -1910,7 +1913,7 @@
     </row>
     <row r="17" spans="1:26" ht="56" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>73</v>
@@ -1934,13 +1937,13 @@
         <v>91</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>23</v>
@@ -1962,7 +1965,7 @@
     </row>
     <row r="18" spans="1:26" ht="70" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>13</v>
@@ -1974,7 +1977,7 @@
         <v>15</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>17</v>
@@ -1983,13 +1986,13 @@
         <v>18</v>
       </c>
       <c r="H18" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>30</v>
@@ -2014,7 +2017,7 @@
     </row>
     <row r="19" spans="1:26" ht="112" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>73</v>
@@ -2026,7 +2029,7 @@
         <v>15</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>17</v>
@@ -2035,16 +2038,16 @@
         <v>18</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>29</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>23</v>
@@ -2066,7 +2069,7 @@
     </row>
     <row r="20" spans="1:26" ht="56" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>13</v>
@@ -2078,7 +2081,7 @@
         <v>15</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>20</v>
@@ -2087,13 +2090,13 @@
         <v>18</v>
       </c>
       <c r="H20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>23</v>
@@ -29581,68 +29584,68 @@
     <col min="7" max="7" width="75.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="8" customFormat="1" ht="28" x14ac:dyDescent="0.15">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:25" s="7" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
     </row>
     <row r="2" spans="1:25" ht="126" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -29665,25 +29668,25 @@
     </row>
     <row r="3" spans="1:25" ht="84" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -29706,25 +29709,25 @@
     </row>
     <row r="4" spans="1:25" ht="112" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -29746,26 +29749,26 @@
       <c r="Y4" s="1"/>
     </row>
     <row r="5" spans="1:25" ht="126" x14ac:dyDescent="0.15">
-      <c r="A5" s="4" t="s">
+      <c r="A5" t="s">
         <v>63</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -56663,7 +56666,7 @@
   </sheetPr>
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -56688,80 +56691,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="88" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="4" t="s">
         <v>165</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>166</v>
       </c>
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
@@ -56771,76 +56774,76 @@
         <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>168</v>
       </c>
       <c r="D2" s="3">
         <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>52</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>173</v>
-      </c>
       <c r="O2" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="T2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="Y2" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="13" x14ac:dyDescent="0.15">
@@ -56848,76 +56851,76 @@
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>168</v>
       </c>
       <c r="D3" s="3">
         <v>2</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>52</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="13" x14ac:dyDescent="0.15">
@@ -56925,76 +56928,76 @@
         <v>48</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="H4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="J4" s="2" t="s">
+      <c r="L4" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="S4" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>182</v>
       </c>
       <c r="T4" s="2" t="s">
         <v>20</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="13" x14ac:dyDescent="0.15">
@@ -57002,76 +57005,76 @@
         <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="K5" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="N5" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="H5" s="2" t="s">
+      <c r="O5" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="U5" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="U5" s="2" t="s">
-        <v>172</v>
-      </c>
       <c r="V5" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="13" x14ac:dyDescent="0.15">
@@ -57079,76 +57082,76 @@
         <v>72</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>172</v>
-      </c>
       <c r="J6" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="S6" s="2" t="s">
         <v>18</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Y6" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="13" x14ac:dyDescent="0.15">
@@ -57156,76 +57159,76 @@
         <v>76</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>179</v>
-      </c>
       <c r="E7" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="H7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="J7" s="2" t="s">
+      <c r="L7" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="N7" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="K7" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>190</v>
-      </c>
       <c r="O7" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="S7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Y7" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="13" x14ac:dyDescent="0.15">
@@ -57233,307 +57236,307 @@
         <v>92</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>179</v>
-      </c>
       <c r="E8" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>52</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N8" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="T8" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="O8" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="S8" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="T8" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="U8" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="X8" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Y8" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>172</v>
-      </c>
       <c r="J9" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="S9" s="2" t="s">
         <v>18</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="X9" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Y9" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>179</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G10" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>52</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N10" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="T10" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="O10" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="R10" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="S10" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="T10" s="2" t="s">
-        <v>197</v>
-      </c>
       <c r="U10" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="X10" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Y10" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="13" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>168</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G11" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>52</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="S11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="X11" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Y11" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="13" x14ac:dyDescent="0.15">
@@ -57541,76 +57544,76 @@
         <v>60</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>168</v>
-      </c>
       <c r="D12" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>52</v>
       </c>
       <c r="H12" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>52</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>20</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="S12" s="2" t="s">
         <v>18</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="U12" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="X12" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Y12" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="13" x14ac:dyDescent="0.15">
@@ -57618,153 +57621,153 @@
         <v>24</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>168</v>
-      </c>
       <c r="D13" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>52</v>
       </c>
       <c r="H13" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>52</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="S13" s="2" t="s">
         <v>18</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="X13" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Y13" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>179</v>
-      </c>
       <c r="E14" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F14" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>52</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="S14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="V14" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="X14" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Y14" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="13" x14ac:dyDescent="0.15">
@@ -57772,153 +57775,153 @@
         <v>86</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="H15" s="2" t="s">
+      <c r="K15" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>172</v>
-      </c>
       <c r="L15" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="S15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="V15" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="X15" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Y15" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="13" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="H16" s="2" t="s">
+      <c r="K16" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>172</v>
-      </c>
       <c r="L16" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="S16" s="2" t="s">
         <v>18</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="V16" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="W16" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="X16" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Y16" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="13" x14ac:dyDescent="0.15">
@@ -57926,153 +57929,153 @@
         <v>40</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>179</v>
-      </c>
       <c r="E17" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F17" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="H17" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="I17" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>52</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V17" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="W17" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="X17" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Y17" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>168</v>
-      </c>
       <c r="D18" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>52</v>
       </c>
       <c r="H18" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I18" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>52</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="S18" s="2" t="s">
         <v>18</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="W18" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="X18" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Y18" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" spans="1:25" ht="13" x14ac:dyDescent="0.15">
@@ -58080,55 +58083,55 @@
         <v>63</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>168</v>
-      </c>
       <c r="D19" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G19" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="I19" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>172</v>
-      </c>
       <c r="J19" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="N19" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="K19" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="N19" s="2" t="s">
-        <v>211</v>
-      </c>
       <c r="O19" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="S19" s="2" t="s">
         <v>18</v>
@@ -58137,75 +58140,75 @@
         <v>20</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="V19" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="W19" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="X19" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Y19" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>179</v>
-      </c>
       <c r="E20" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G20" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>171</v>
-      </c>
       <c r="I20" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>52</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="S20" s="2" t="s">
         <v>18</v>
@@ -58214,173 +58217,173 @@
         <v>20</v>
       </c>
       <c r="U20" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="V20" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W20" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="X20" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Y20" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>168</v>
-      </c>
       <c r="D21" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G21" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>171</v>
-      </c>
       <c r="I21" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>52</v>
       </c>
       <c r="K21" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="N21" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="L21" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="N21" s="2" t="s">
+      <c r="O21" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="R21" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="S21" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="O21" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="P21" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q21" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="R21" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="S21" s="2" t="s">
+      <c r="T21" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="T21" s="2" t="s">
+      <c r="U21" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="V21" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="W21" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="X21" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="Y21" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="U21" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="V21" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="W21" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="X21" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="Y21" s="2" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>168</v>
-      </c>
       <c r="D22" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G22" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>171</v>
-      </c>
       <c r="I22" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>52</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="U22" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="V22" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W22" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="X22" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Y22" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="23" spans="1:25" ht="13" x14ac:dyDescent="0.15">
@@ -58391,13 +58394,13 @@
     </row>
     <row r="25" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D26" s="3"/>
     </row>

</xml_diff>